<commit_message>
updated targets and bau
</commit_message>
<xml_diff>
--- a/data-raw/model_data/targets.xlsx
+++ b/data-raw/model_data/targets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lffox/Dropbox (Grattan Institute)/Transport Program/Project - Electric vehicles/Analysis/fleeteffSim/data-raw/model_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F983D20-BA99-9E40-B47D-5A5883194AAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A877C24F-8E74-5F4F-A0CA-022242CD7E5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{8B27FF0C-4EF2-3749-AB9A-861A4F7E9CE0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21020" xr2:uid="{8B27FF0C-4EF2-3749-AB9A-861A4F7E9CE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,10 +129,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -434,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52943D3-D443-1C46-B8C5-1FA463E1C284}">
   <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,7 +705,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -727,7 +723,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -745,7 +741,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -763,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -781,7 +777,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -799,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -817,7 +813,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -835,7 +831,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -853,7 +849,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -871,7 +867,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -889,7 +885,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="3">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -907,7 +903,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="3">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -925,7 +921,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="3">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -943,7 +939,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="3">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -961,7 +957,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -1219,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -1238,7 +1234,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -1257,7 +1253,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -1276,7 +1272,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -1287,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -1298,7 +1294,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1309,7 +1305,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1320,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1331,7 +1327,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1342,7 +1338,7 @@
         <v>1</v>
       </c>
       <c r="C52" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1353,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="C53" s="2">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1364,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1375,7 +1371,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="2">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1386,7 +1382,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="2">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1397,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="2">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1551,7 +1547,7 @@
         <v>2</v>
       </c>
       <c r="C71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1562,7 +1558,7 @@
         <v>2</v>
       </c>
       <c r="C72" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1573,7 +1569,7 @@
         <v>2</v>
       </c>
       <c r="C73" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1584,7 +1580,7 @@
         <v>2</v>
       </c>
       <c r="C74" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -1595,7 +1591,7 @@
         <v>2</v>
       </c>
       <c r="C75" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -1606,7 +1602,7 @@
         <v>2</v>
       </c>
       <c r="C76" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -1617,7 +1613,7 @@
         <v>2</v>
       </c>
       <c r="C77" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -1628,7 +1624,7 @@
         <v>2</v>
       </c>
       <c r="C78" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -1639,7 +1635,7 @@
         <v>2</v>
       </c>
       <c r="C79" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1650,7 +1646,7 @@
         <v>2</v>
       </c>
       <c r="C80" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -1661,7 +1657,7 @@
         <v>2</v>
       </c>
       <c r="C81" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -1672,7 +1668,7 @@
         <v>2</v>
       </c>
       <c r="C82" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -1683,7 +1679,7 @@
         <v>2</v>
       </c>
       <c r="C83" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -1694,7 +1690,7 @@
         <v>2</v>
       </c>
       <c r="C84" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -1705,7 +1701,7 @@
         <v>2</v>
       </c>
       <c r="C85" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>